<commit_message>
calculated portion of tests executed
</commit_message>
<xml_diff>
--- a/data/csv/results/charts-tables.xlsx
+++ b/data/csv/results/charts-tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tdao/vt-2023/sbfl-study/data/csv/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{775D3C04-4D35-7744-B2B1-5714BBCE39CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F90FDC6-1465-764A-8B1B-119C6AF717D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1340" yWindow="1460" windowWidth="32220" windowHeight="19280" activeTab="6" xr2:uid="{FE8ACBDC-0703-A34E-809D-952EBA7EFD33}"/>
+    <workbookView xWindow="960" yWindow="760" windowWidth="32220" windowHeight="19280" activeTab="3" xr2:uid="{FE8ACBDC-0703-A34E-809D-952EBA7EFD33}"/>
   </bookViews>
   <sheets>
     <sheet name="Ranked By Algorithms" sheetId="8" r:id="rId1"/>
@@ -223,7 +223,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="130">
   <si>
     <t xml:space="preserve"> Top 5(#)</t>
   </si>
@@ -608,6 +608,12 @@
   <si>
     <t># of passed Tests</t>
   </si>
+  <si>
+    <t>Portion of Tests Executed (%)[R]</t>
+  </si>
+  <si>
+    <t>Portion of Tests Executed (%)[I]</t>
+  </si>
 </sst>
 </file>
 
@@ -689,7 +695,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -713,6 +719,27 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -13842,16 +13869,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>393700</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>127000</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>812800</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -13880,7 +13907,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6692900" y="25400"/>
+          <a:off x="8763000" y="0"/>
           <a:ext cx="7162800" cy="1346200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -13897,16 +13924,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>393700</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>97451</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -13935,8 +13962,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6527800" y="0"/>
-          <a:ext cx="5715000" cy="1511300"/>
+          <a:off x="8928100" y="0"/>
+          <a:ext cx="8724900" cy="2307251"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13952,16 +13979,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>88900</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>98206</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -13990,8 +14017,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7315200" y="0"/>
-          <a:ext cx="5372100" cy="3340100"/>
+          <a:off x="9994900" y="0"/>
+          <a:ext cx="8369300" cy="5203606"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14940,7 +14967,7 @@
   <dimension ref="A1:Y27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:XFD22"/>
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16929,7 +16956,7 @@
   <dimension ref="A1:Y18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18249,10 +18276,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2B32840-DF8F-6347-96CC-367B9BABC7F9}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18266,9 +18293,11 @@
     <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.83203125" style="20" customWidth="1"/>
+    <col min="11" max="11" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>108</v>
       </c>
@@ -18296,8 +18325,14 @@
       <c r="I1" s="9" t="s">
         <v>116</v>
       </c>
+      <c r="J1" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="K1" s="22" t="s">
+        <v>128</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>97</v>
       </c>
@@ -18325,8 +18360,14 @@
       <c r="I2" s="10">
         <v>20</v>
       </c>
+      <c r="J2" s="21">
+        <v>0.39</v>
+      </c>
+      <c r="K2" s="23">
+        <v>0.44</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>93</v>
       </c>
@@ -18353,6 +18394,12 @@
       </c>
       <c r="I3" s="10">
         <v>22</v>
+      </c>
+      <c r="J3" s="21">
+        <v>1</v>
+      </c>
+      <c r="K3" s="23">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -18363,10 +18410,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE616C87-8848-5249-8B41-9938EB2CF411}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18380,9 +18427,11 @@
     <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.33203125" customWidth="1"/>
+    <col min="11" max="11" width="17.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>117</v>
       </c>
@@ -18410,8 +18459,14 @@
       <c r="I1" s="9" t="s">
         <v>116</v>
       </c>
+      <c r="J1" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="K1" s="26" t="s">
+        <v>128</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -18439,8 +18494,14 @@
       <c r="I2" s="10">
         <v>20</v>
       </c>
+      <c r="J2" s="25">
+        <v>0.39</v>
+      </c>
+      <c r="K2" s="27">
+        <v>0.44</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -18468,8 +18529,14 @@
       <c r="I3" s="10">
         <v>19</v>
       </c>
+      <c r="J3" s="25">
+        <v>0.48</v>
+      </c>
+      <c r="K3" s="27">
+        <v>0.54</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -18497,8 +18564,14 @@
       <c r="I4" s="10">
         <v>18</v>
       </c>
+      <c r="J4" s="25">
+        <v>0.62</v>
+      </c>
+      <c r="K4" s="27">
+        <v>0.55000000000000004</v>
+      </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -18526,8 +18599,14 @@
       <c r="I5" s="10">
         <v>23</v>
       </c>
+      <c r="J5" s="25">
+        <v>0.83</v>
+      </c>
+      <c r="K5" s="27">
+        <v>0.56999999999999995</v>
+      </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -18554,6 +18633,12 @@
       </c>
       <c r="I6" s="10">
         <v>21</v>
+      </c>
+      <c r="J6" s="25">
+        <v>0.93</v>
+      </c>
+      <c r="K6" s="27">
+        <v>0.56999999999999995</v>
       </c>
     </row>
   </sheetData>
@@ -18564,10 +18649,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CCF01EA-F85A-BB40-AC5E-712240C683F5}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18581,9 +18666,11 @@
     <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.1640625" customWidth="1"/>
+    <col min="11" max="11" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>118</v>
       </c>
@@ -18611,8 +18698,14 @@
       <c r="I1" s="9" t="s">
         <v>116</v>
       </c>
+      <c r="J1" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="K1" s="26" t="s">
+        <v>128</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -18640,8 +18733,14 @@
       <c r="I2" s="10">
         <v>20</v>
       </c>
+      <c r="J2" s="17">
+        <v>0.41</v>
+      </c>
+      <c r="K2" s="27">
+        <v>0.46</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -18669,8 +18768,14 @@
       <c r="I3" s="10">
         <v>21</v>
       </c>
+      <c r="J3" s="17">
+        <v>0.44</v>
+      </c>
+      <c r="K3" s="27">
+        <v>0.47</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -18698,8 +18803,14 @@
       <c r="I4" s="10">
         <v>21</v>
       </c>
+      <c r="J4" s="17">
+        <v>0.46</v>
+      </c>
+      <c r="K4" s="27">
+        <v>0.48</v>
+      </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -18727,8 +18838,14 @@
       <c r="I5" s="10">
         <v>21</v>
       </c>
+      <c r="J5" s="17">
+        <v>0.46</v>
+      </c>
+      <c r="K5" s="27">
+        <v>0.48</v>
+      </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -18756,8 +18873,14 @@
       <c r="I6" s="10">
         <v>20</v>
       </c>
+      <c r="J6" s="17">
+        <v>0.48</v>
+      </c>
+      <c r="K6" s="27">
+        <v>0.48</v>
+      </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -18785,8 +18908,14 @@
       <c r="I7" s="10">
         <v>20</v>
       </c>
+      <c r="J7" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="K7" s="27">
+        <v>0.48</v>
+      </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -18814,8 +18943,14 @@
       <c r="I8" s="10">
         <v>21</v>
       </c>
+      <c r="J8" s="17">
+        <v>0.52</v>
+      </c>
+      <c r="K8" s="27">
+        <v>0.49</v>
+      </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -18843,8 +18978,14 @@
       <c r="I9" s="10">
         <v>21</v>
       </c>
+      <c r="J9" s="17">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="K9" s="27">
+        <v>0.5</v>
+      </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -18872,8 +19013,14 @@
       <c r="I10" s="10">
         <v>20</v>
       </c>
+      <c r="J10" s="17">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="K10" s="27">
+        <v>0.49</v>
+      </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -18900,6 +19047,12 @@
       </c>
       <c r="I11" s="10">
         <v>22</v>
+      </c>
+      <c r="J11" s="17">
+        <v>0.54</v>
+      </c>
+      <c r="K11" s="27">
+        <v>0.49</v>
       </c>
     </row>
   </sheetData>
@@ -20432,7 +20585,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B487A7C-88E7-904E-A873-C5A5747EF4B6}">
   <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N73" sqref="N73"/>
     </sheetView>
   </sheetViews>
@@ -21126,7 +21279,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05BEC728-C1D2-F348-A258-F8D57E467B19}">
   <dimension ref="A1:E83"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Y64" sqref="Y64"/>
     </sheetView>
   </sheetViews>

</xml_diff>